<commit_message>
Excel Template with Tags :godmode:
</commit_message>
<xml_diff>
--- a/Templates/RSL-IL4Privacy-ExcelTemplate.xlsx
+++ b/Templates/RSL-IL4Privacy-ExcelTemplate.xlsx
@@ -30,13 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="107">
-  <si>
-    <t>We collect the content and other information you provide when you use our Services, including when you sign up for an account, create or share, and message or communicate with others. This can include the location of a photo or the date a file was created.</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/policy.php</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="120">
   <si>
     <t>Disclosure</t>
   </si>
@@ -68,9 +62,6 @@
     <t>statements (id)</t>
   </si>
   <si>
-    <t>Facebook Account</t>
-  </si>
-  <si>
     <t>Usage Information</t>
   </si>
   <si>
@@ -80,28 +71,10 @@
     <t>Tool</t>
   </si>
   <si>
-    <t>Activity Log tool</t>
-  </si>
-  <si>
-    <t>Users are able to manage the content and information shared when using Facebook</t>
-  </si>
-  <si>
-    <t>Users must accept Statement of Rights and Responsibilities (including Data Policy)</t>
-  </si>
-  <si>
     <t>Informative</t>
   </si>
   <si>
     <t>attributes</t>
-  </si>
-  <si>
-    <t>first name,
-surname,
-email,
-mobile number,
-password,
-date of birth,
-gender</t>
   </si>
   <si>
     <t>PrivateData (id)</t>
@@ -114,9 +87,6 @@
     <t>Action</t>
   </si>
   <si>
-    <t>1, 4, 5, 6, 7</t>
-  </si>
-  <si>
     <t>organization</t>
   </si>
   <si>
@@ -312,21 +282,6 @@
     <t>forbidden</t>
   </si>
   <si>
-    <t>Facebook services owner</t>
-  </si>
-  <si>
-    <t>Description of generic statements equal to the sub-services descriptions combined or write general description? DEAL LATER</t>
-  </si>
-  <si>
-    <t>Account</t>
-  </si>
-  <si>
-    <t>manage account</t>
-  </si>
-  <si>
-    <t>Services with sub-services are not supposed to be used in Eddy; use sub-services instead</t>
-  </si>
-  <si>
     <t>Index</t>
   </si>
   <si>
@@ -358,6 +313,84 @@
   </si>
   <si>
     <t>Period (only for type=Retention)</t>
+  </si>
+  <si>
+    <t>SDescription</t>
+  </si>
+  <si>
+    <t>SId</t>
+  </si>
+  <si>
+    <t>SPDId</t>
+  </si>
+  <si>
+    <t>SRId</t>
+  </si>
+  <si>
+    <t>SSId</t>
+  </si>
+  <si>
+    <t>RId</t>
+  </si>
+  <si>
+    <t>RDescription</t>
+  </si>
+  <si>
+    <t>StCondition</t>
+  </si>
+  <si>
+    <t>StPDId</t>
+  </si>
+  <si>
+    <t>StRId</t>
+  </si>
+  <si>
+    <t>StSId</t>
+  </si>
+  <si>
+    <t>StEId</t>
+  </si>
+  <si>
+    <t>StPeriod</t>
+  </si>
+  <si>
+    <t>StModality</t>
+  </si>
+  <si>
+    <t>StType</t>
+  </si>
+  <si>
+    <t>RScope</t>
+  </si>
+  <si>
+    <t>RType</t>
+  </si>
+  <si>
+    <t>SName</t>
+  </si>
+  <si>
+    <t>PDId</t>
+  </si>
+  <si>
+    <t>PDType</t>
+  </si>
+  <si>
+    <t>PDDescription</t>
+  </si>
+  <si>
+    <t>PDAttributes</t>
+  </si>
+  <si>
+    <t>EId</t>
+  </si>
+  <si>
+    <t>EName</t>
+  </si>
+  <si>
+    <t>EDescription</t>
+  </si>
+  <si>
+    <t>EType</t>
   </si>
 </sst>
 </file>
@@ -405,7 +438,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -421,12 +454,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -561,7 +588,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -617,9 +644,16 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperligação" xfId="1" builtinId="8"/>
@@ -963,51 +997,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21">
-      <c r="A1" s="28" t="s">
-        <v>102</v>
-      </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
+      <c r="A1" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
     </row>
     <row r="2" spans="1:4" ht="21">
-      <c r="A2" s="29" t="s">
-        <v>96</v>
+      <c r="A2" s="28" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1030,7 +1064,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1049,84 +1083,77 @@
   <sheetData>
     <row r="1" spans="1:10" ht="30">
       <c r="A1" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="14" t="s">
+      <c r="D1" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="E1" s="15" t="s">
-        <v>10</v>
-      </c>
       <c r="F1" s="15" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="G1" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="J1" s="24" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D2" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="E2" s="29" t="s">
+        <v>108</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H2" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="I2" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="J1" s="24" t="s">
+      <c r="J2" s="3" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="30">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="3">
-        <v>1</v>
-      </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3">
-        <v>1</v>
-      </c>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-    </row>
     <row r="5" spans="1:10">
-      <c r="B5" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="B5" s="2"/>
     </row>
   </sheetData>
   <sortState ref="A2:F92">
     <sortCondition ref="E2:E92" customList="Collection,Disclosure,Retention,Usage,Informative"/>
   </sortState>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2">
-      <formula1>statements_type</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2">
-      <formula1 xml:space="preserve"> modality_type</formula1>
-    </dataValidation>
-  </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1135,7 +1162,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD12"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1148,45 +1175,39 @@
   <sheetData>
     <row r="1" spans="1:5" ht="29.25" customHeight="1">
       <c r="A1" s="13" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E1" s="24" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="25" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="25">
-        <v>1</v>
-      </c>
       <c r="B2" s="8" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>27</v>
+        <v>109</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="3"/>
+        <v>110</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>97</v>
+      </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C2">
-      <formula1>recipient_scope</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D2">
-      <formula1>recipient_type</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -1197,7 +1218,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1209,45 +1230,40 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="13" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D1" s="23" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E1" s="23" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1">
-      <c r="A2" s="25">
-        <v>1</v>
+      <c r="A2" s="25" t="s">
+        <v>95</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>93</v>
+        <v>111</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>94</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="B6" t="s">
-        <v>92</v>
+        <v>96</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="B9" s="26" t="s">
-        <v>95</v>
-      </c>
+      <c r="B9" s="30"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1260,12 +1276,12 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD9"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.140625" customWidth="1"/>
+    <col min="1" max="1" width="5.5703125" customWidth="1"/>
     <col min="2" max="2" width="19.7109375" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
     <col min="4" max="4" width="37" customWidth="1"/>
@@ -1273,38 +1289,33 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="13" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="105.75" customHeight="1">
-      <c r="A2" s="5">
-        <v>1</v>
+      <c r="A2" s="5" t="s">
+        <v>112</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>14</v>
+        <v>113</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>12</v>
+        <v>114</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>21</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B2">
-      <formula1>privatedata_type</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1314,7 +1325,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD6"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1327,38 +1338,33 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="13" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="5">
-        <v>1</v>
+      <c r="A2" s="5" t="s">
+        <v>116</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>16</v>
+        <v>117</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>17</v>
+        <v>118</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>15</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D2">
-      <formula1>enforcement_type</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -1385,367 +1391,367 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18.75">
       <c r="A1" s="12" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="13" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="16" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="16" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="16" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="16" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="19" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="18.75">
       <c r="A9" s="12" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="13" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="16" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="16" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="16" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="16" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="30">
       <c r="A15" s="22" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="19" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="18.75">
       <c r="A18" s="12" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B18" s="11"/>
       <c r="C18" s="11"/>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="13" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="16" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="16" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="16" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="19" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B23" s="20" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C23" s="21" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="19" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="B24" s="20" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="18.75">
       <c r="A26" s="12" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B26" s="11"/>
       <c r="C26" s="11"/>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="13" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="16" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="16" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="16" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C30" s="18" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="19" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B31" s="20" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C31" s="21" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="18.75">
       <c r="A33" s="12" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B33" s="11"/>
       <c r="C33" s="11"/>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="13" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B34" s="14" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="16" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="16" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C36" s="18" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="16" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="C37" s="18" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="16" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="C38" s="18" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="19" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B39" s="20" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C39" s="21" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1771,95 +1777,95 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
       <c r="F1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="E5" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="F5" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B6" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="C6" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D6" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed the Excel template
</commit_message>
<xml_diff>
--- a/Templates/RSL-IL4Privacy-ExcelTemplate.xlsx
+++ b/Templates/RSL-IL4Privacy-ExcelTemplate.xlsx
@@ -1067,10 +1067,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1150,9 +1150,6 @@
       <c r="J2" s="3" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="B5" s="2"/>
     </row>
   </sheetData>
   <sortState ref="A2:F92">

</xml_diff>

<commit_message>
Excel gen with metadata info
</commit_message>
<xml_diff>
--- a/Templates/RSL-IL4Privacy-ExcelTemplate.xlsx
+++ b/Templates/RSL-IL4Privacy-ExcelTemplate.xlsx
@@ -4,32 +4,33 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7980" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7980"/>
   </bookViews>
   <sheets>
-    <sheet name="Index" sheetId="8" r:id="rId1"/>
-    <sheet name="Statements" sheetId="1" r:id="rId2"/>
-    <sheet name="Recipients" sheetId="5" r:id="rId3"/>
-    <sheet name="Services" sheetId="2" r:id="rId4"/>
-    <sheet name="PrivateData" sheetId="3" r:id="rId5"/>
-    <sheet name="Enforcements" sheetId="4" r:id="rId6"/>
-    <sheet name="Configuration Types" sheetId="6" r:id="rId7"/>
-    <sheet name="Script Data" sheetId="7" r:id="rId8"/>
+    <sheet name="Home" sheetId="9" r:id="rId1"/>
+    <sheet name="Index" sheetId="8" r:id="rId2"/>
+    <sheet name="Statements" sheetId="1" r:id="rId3"/>
+    <sheet name="Recipients" sheetId="5" r:id="rId4"/>
+    <sheet name="Services" sheetId="2" r:id="rId5"/>
+    <sheet name="PrivateData" sheetId="3" r:id="rId6"/>
+    <sheet name="Enforcements" sheetId="4" r:id="rId7"/>
+    <sheet name="Configuration Types" sheetId="6" r:id="rId8"/>
+    <sheet name="Script Data" sheetId="7" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="enforcement_type" localSheetId="5">'Script Data'!$B$5:$F$5</definedName>
-    <definedName name="modality_type" localSheetId="1">'Script Data'!$B$6:$D$6</definedName>
-    <definedName name="privatedata_type" localSheetId="4">'Script Data'!$B$4:$C$4</definedName>
-    <definedName name="recipient_scope" localSheetId="2">'Script Data'!$B$2:$D$2</definedName>
-    <definedName name="recipient_type" localSheetId="2">'Script Data'!$B$3:$D$3</definedName>
-    <definedName name="statements_type" localSheetId="1">'Script Data'!$B$1:$F$1</definedName>
+    <definedName name="enforcement_type" localSheetId="6">'Script Data'!$B$5:$F$5</definedName>
+    <definedName name="modality_type" localSheetId="2">'Script Data'!$B$6:$D$6</definedName>
+    <definedName name="privatedata_type" localSheetId="5">'Script Data'!$B$4:$C$4</definedName>
+    <definedName name="recipient_scope" localSheetId="3">'Script Data'!$B$2:$D$2</definedName>
+    <definedName name="recipient_type" localSheetId="3">'Script Data'!$B$3:$D$3</definedName>
+    <definedName name="statements_type" localSheetId="2">'Script Data'!$B$1:$F$1</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="132">
   <si>
     <t>Disclosure</t>
   </si>
@@ -402,6 +403,30 @@
   </si>
   <si>
     <t>Enforcements</t>
+  </si>
+  <si>
+    <t>Author(s)</t>
+  </si>
+  <si>
+    <t>Organization(s)</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>HOrganizations</t>
+  </si>
+  <si>
+    <t>HDate</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>HVersion</t>
+  </si>
+  <si>
+    <t>HAuthors</t>
   </si>
 </sst>
 </file>
@@ -599,7 +624,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -664,6 +689,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperligação" xfId="1" builtinId="8"/>
@@ -995,10 +1021,70 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="21">
+      <c r="A1" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="31" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="B3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="31" t="s">
+        <v>126</v>
+      </c>
+      <c r="B4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="31" t="s">
+        <v>129</v>
+      </c>
+      <c r="B5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1069,11 +1155,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1164,7 +1250,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -1220,7 +1306,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -1275,7 +1361,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1324,7 +1410,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1374,7 +1460,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C39"/>
   <sheetViews>
@@ -1764,7 +1850,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F6"/>
   <sheetViews>

</xml_diff>

<commit_message>
PolicyName & Description added to metadata
</commit_message>
<xml_diff>
--- a/Templates/RSL-IL4Privacy-ExcelTemplate.xlsx
+++ b/Templates/RSL-IL4Privacy-ExcelTemplate.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="135">
   <si>
     <t>Disclosure</t>
   </si>
@@ -427,6 +427,15 @@
   </si>
   <si>
     <t>HAuthors</t>
+  </si>
+  <si>
+    <t>Policy Name</t>
+  </si>
+  <si>
+    <t>HDescription</t>
+  </si>
+  <si>
+    <t>HPolicyName</t>
   </si>
 </sst>
 </file>
@@ -1021,7 +1030,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -1043,33 +1052,49 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="31" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="B2" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="31" t="s">
-        <v>125</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="31" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B4" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="B5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="31" t="s">
+        <v>126</v>
+      </c>
+      <c r="B6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="31" t="s">
         <v>129</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B7" t="s">
         <v>130</v>
       </c>
     </row>

</xml_diff>